<commit_message>
adding some figure, adding noue filter, adding more than 1 occurences filter, fixing Nicolas Rolen classification
</commit_message>
<xml_diff>
--- a/data/Base de données anti trans.xlsx
+++ b/data/Base de données anti trans.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="493">
   <si>
     <t>ID ASSO</t>
   </si>
@@ -6703,9 +6703,6 @@
     <t>Nationaliste, Identitaire</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>ISSEP</t>
   </si>
   <si>
@@ -6954,7 +6951,7 @@
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6972,12 +6969,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000ff"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -7047,7 +7038,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -7079,7 +7070,7 @@
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
@@ -7091,25 +7082,19 @@
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -7521,24 +7506,22 @@
       <c r="F4" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="G4" s="18" t="s">
-        <v>413</v>
-      </c>
+      <c r="G4" s="18"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="19"/>
+      <c r="I4" s="18"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>414</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>416</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>409</v>
@@ -7546,9 +7529,7 @@
       <c r="F5" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="G5" s="20" t="s">
-        <v>413</v>
-      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="6"/>
       <c r="I5" s="2"/>
     </row>
@@ -7556,23 +7537,23 @@
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="18" t="s">
+        <v>416</v>
+      </c>
+      <c r="C6" s="19" t="s">
         <v>417</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="D6" s="18" t="s">
         <v>418</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>419</v>
-      </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="18" t="s">
         <v>409</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>405</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H6" s="6"/>
       <c r="I6" s="2"/>
@@ -7582,10 +7563,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>421</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>422</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>403</v>
@@ -7596,9 +7577,7 @@
       <c r="F7" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="G7" s="20" t="s">
-        <v>413</v>
-      </c>
+      <c r="G7" s="2"/>
       <c r="H7" s="6"/>
       <c r="I7" s="2"/>
     </row>
@@ -7607,13 +7586,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>423</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>424</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>409</v>
@@ -7621,9 +7600,7 @@
       <c r="F8" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="G8" s="20" t="s">
-        <v>413</v>
-      </c>
+      <c r="G8" s="2"/>
       <c r="H8" s="6"/>
       <c r="I8" s="2"/>
     </row>
@@ -7632,13 +7609,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="C9" s="15" t="s">
         <v>425</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="D9" s="2" t="s">
         <v>426</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>427</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>409</v>
@@ -7646,9 +7623,7 @@
       <c r="F9" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="G9" s="20" t="s">
-        <v>413</v>
-      </c>
+      <c r="G9" s="2"/>
       <c r="H9" s="6"/>
       <c r="I9" s="2"/>
     </row>
@@ -7657,10 +7632,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>428</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>429</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>403</v>
@@ -7680,19 +7655,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>430</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="D11" s="2" t="s">
         <v>431</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>433</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>434</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -7702,17 +7677,17 @@
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="18" t="s">
+        <v>434</v>
+      </c>
+      <c r="C12" s="19" t="s">
         <v>435</v>
       </c>
-      <c r="C12" s="21" t="s">
+      <c r="D12" s="18" t="s">
         <v>436</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="E12" s="18" t="s">
         <v>437</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>438</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>405</v>
@@ -7725,23 +7700,23 @@
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="18" t="s">
+        <v>438</v>
+      </c>
+      <c r="C13" s="19" t="s">
         <v>439</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="D13" s="18" t="s">
         <v>440</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="E13" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>433</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>442</v>
       </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -7750,20 +7725,20 @@
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
+        <v>442</v>
+      </c>
+      <c r="C14" s="19" t="s">
         <v>443</v>
       </c>
-      <c r="C14" s="21" t="s">
-        <v>444</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>441</v>
-      </c>
-      <c r="E14" s="19" t="s">
+      <c r="D14" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>433</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>434</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="2"/>
@@ -7774,28 +7749,26 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>445</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="2" t="s">
         <v>446</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>433</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>413</v>
-      </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>449</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
@@ -7803,13 +7776,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>450</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="D16" s="2" t="s">
         <v>451</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>452</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>404</v>
@@ -7826,13 +7799,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>453</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>455</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>404</v>
@@ -7840,9 +7813,7 @@
       <c r="F17" s="2" t="s">
         <v>405</v>
       </c>
-      <c r="G17" s="20" t="s">
-        <v>413</v>
-      </c>
+      <c r="G17" s="2"/>
       <c r="H17" s="6"/>
       <c r="I17" s="2"/>
     </row>
@@ -7850,23 +7821,23 @@
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="18" t="s">
+        <v>455</v>
+      </c>
+      <c r="C18" s="19" t="s">
         <v>456</v>
       </c>
-      <c r="C18" s="21" t="s">
-        <v>457</v>
-      </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="G18" s="2" t="s">
         <v>441</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>433</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>442</v>
       </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -7875,23 +7846,23 @@
       <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="18" t="s">
+        <v>457</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>458</v>
       </c>
-      <c r="C19" s="21" t="s">
+      <c r="D19" s="18" t="s">
         <v>459</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="E19" s="18" t="s">
         <v>460</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="F19" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>461</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>462</v>
       </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
@@ -7901,19 +7872,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="C20" s="15" t="s">
         <v>463</v>
       </c>
-      <c r="C20" s="15" t="s">
-        <v>464</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>433</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
@@ -7923,23 +7894,23 @@
       <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="18" t="s">
+        <v>464</v>
+      </c>
+      <c r="C21" s="19" t="s">
         <v>465</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="D21" s="18" t="s">
         <v>466</v>
       </c>
-      <c r="D21" s="19" t="s">
-        <v>467</v>
-      </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>434</v>
-      </c>
       <c r="G21" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H21" s="6"/>
       <c r="I21" s="2"/>
@@ -7948,20 +7919,20 @@
       <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="18" t="s">
+        <v>467</v>
+      </c>
+      <c r="C22" s="19" t="s">
         <v>468</v>
       </c>
-      <c r="C22" s="21" t="s">
-        <v>469</v>
-      </c>
-      <c r="D22" s="19" t="s">
-        <v>441</v>
-      </c>
-      <c r="E22" s="19" t="s">
+      <c r="D22" s="18" t="s">
+        <v>440</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>432</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>433</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>434</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="2"/>
@@ -7972,23 +7943,21 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C23" s="15" t="s">
         <v>470</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="D23" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>472</v>
-      </c>
       <c r="E23" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>413</v>
-      </c>
+        <v>433</v>
+      </c>
+      <c r="G23" s="2"/>
       <c r="H23" s="6"/>
       <c r="I23" s="2"/>
     </row>
@@ -7996,23 +7965,23 @@
       <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="18" t="s">
+        <v>472</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>473</v>
       </c>
-      <c r="C24" s="21" t="s">
-        <v>474</v>
-      </c>
-      <c r="D24" s="19" t="s">
-        <v>472</v>
+      <c r="D24" s="18" t="s">
+        <v>471</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -8022,13 +7991,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C25" s="15" t="s">
         <v>475</v>
       </c>
-      <c r="C25" s="15" t="s">
-        <v>476</v>
-      </c>
       <c r="D25" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>409</v>
@@ -8045,13 +8014,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>477</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="D26" s="2" t="s">
         <v>478</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>479</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>409</v>
@@ -8068,13 +8037,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>480</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="D27" s="2" t="s">
         <v>481</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>482</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>409</v>
@@ -8091,13 +8060,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C28" s="15" t="s">
         <v>483</v>
       </c>
-      <c r="C28" s="15" t="s">
-        <v>484</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>409</v>
@@ -8114,13 +8083,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>484</v>
+      </c>
+      <c r="C29" s="15" t="s">
         <v>485</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>486</v>
-      </c>
       <c r="D29" s="2" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>409</v>
@@ -8137,13 +8106,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="C30" s="15" t="s">
         <v>487</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="D30" s="2" t="s">
         <v>488</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>489</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>409</v>
@@ -8159,16 +8128,16 @@
       <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="18" t="s">
+        <v>489</v>
+      </c>
+      <c r="C31" s="19" t="s">
         <v>490</v>
       </c>
-      <c r="C31" s="21" t="s">
-        <v>491</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>416</v>
-      </c>
-      <c r="E31" s="19" t="s">
+      <c r="D31" s="18" t="s">
+        <v>415</v>
+      </c>
+      <c r="E31" s="18" t="s">
         <v>409</v>
       </c>
       <c r="F31" s="2" t="s">
@@ -8182,16 +8151,16 @@
       <c r="A32" s="3">
         <v>31</v>
       </c>
-      <c r="B32" s="19" t="s">
+      <c r="B32" s="18" t="s">
+        <v>491</v>
+      </c>
+      <c r="C32" s="19" t="s">
         <v>492</v>
       </c>
-      <c r="C32" s="21" t="s">
-        <v>493</v>
-      </c>
-      <c r="D32" s="19" t="s">
+      <c r="D32" s="18" t="s">
         <v>408</v>
       </c>
-      <c r="E32" s="19" t="s">
+      <c r="E32" s="18" t="s">
         <v>404</v>
       </c>
       <c r="F32" s="2" t="s">

</xml_diff>